<commit_message>
added HELLP PATIENT for HELLP syndrome lab events
</commit_message>
<xml_diff>
--- a/protempa-test-suite/src/test/resources/dsb/sample-data.xlsx
+++ b/protempa-test-suite/src/test/resources/dsb/sample-data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="7" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="944" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="776" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="patient" sheetId="1" state="visible" r:id="rId2"/>
@@ -8646,7 +8646,7 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -10466,8 +10466,8 @@
   </sheetPr>
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A25" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A22" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B46" activeCellId="0" pane="topLeft" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -11497,7 +11497,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="0" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C45" s="0" t="n">
         <v>105</v>
@@ -11535,7 +11535,7 @@
   </sheetPr>
   <dimension ref="A1:D106"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A106" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A13" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A106" activeCellId="0" pane="topLeft" sqref="A106"/>
     </sheetView>
   </sheetViews>
@@ -17633,7 +17633,7 @@
   </sheetPr>
   <dimension ref="A1:H231"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A198" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A204" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="E223" activeCellId="0" pane="topLeft" sqref="E223"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix logic for handling propositions with a non-null delete date.
</commit_message>
<xml_diff>
--- a/protempa-test-suite/src/test/resources/dsb/sample-data.xlsx
+++ b/protempa-test-suite/src/test/resources/dsb/sample-data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26709"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arpost/NetBeansProjects/protempa/protempa-test-suite/src/test/resources/dsb/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918E5C98-55D4-A349-BAD0-5442F7BCB674}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9940" yWindow="1280" windowWidth="31540" windowHeight="24480" tabRatio="537" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="537" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="patient" sheetId="1" r:id="rId1"/>
@@ -28,7 +29,7 @@
     <definedName name="_FilterDatabase_1_1" localSheetId="2">encounter!$A$1:$G$2556</definedName>
     <definedName name="_FilterDatabase_1_1_1" localSheetId="2">encounter!$A$1:$G$2556</definedName>
   </definedNames>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="140001" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -6133,7 +6134,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
@@ -6221,6 +6222,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -6547,7 +6551,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7102,7 +7106,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9190,10 +9194,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -10973,14 +10977,14 @@
       <c r="K63" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G2556"/>
+  <autoFilter ref="A1:G2556" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13037,7 +13041,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15284,7 +15288,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K231"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21843,11 +21847,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19:K28"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="L114" sqref="L114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -25073,7 +25077,9 @@
         <v>42425.375</v>
       </c>
       <c r="J114" s="6"/>
-      <c r="K114" s="6"/>
+      <c r="K114" s="6">
+        <v>25569</v>
+      </c>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
@@ -25101,7 +25107,9 @@
         <v>42425.375</v>
       </c>
       <c r="J115" s="6"/>
-      <c r="K115" s="6"/>
+      <c r="K115" s="6">
+        <v>25569</v>
+      </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
@@ -25721,6 +25729,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remove extra column with no data in the encounter tab. Set a delete date for two vital sign records.
</commit_message>
<xml_diff>
--- a/protempa-test-suite/src/test/resources/dsb/sample-data.xlsx
+++ b/protempa-test-suite/src/test/resources/dsb/sample-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arpost/NetBeansProjects/protempa/protempa-test-suite/src/test/resources/dsb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918E5C98-55D4-A349-BAD0-5442F7BCB674}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{377A76D0-6E21-434F-A152-25CD8BEA80FB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="537" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="537" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="patient" sheetId="1" r:id="rId1"/>
@@ -9195,20 +9195,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K63"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="8" max="8" width="23.5" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10.83203125" style="5"/>
+    <col min="7" max="7" width="34.83203125" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>274</v>
       </c>
@@ -9230,17 +9230,17 @@
       <c r="G1" s="1" t="s">
         <v>278</v>
       </c>
+      <c r="H1" s="5" t="s">
+        <v>2027</v>
+      </c>
       <c r="I1" s="5" t="s">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>2028</v>
-      </c>
-      <c r="K1" s="5" t="s">
         <v>2029</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -9262,13 +9262,13 @@
       <c r="G2" t="s">
         <v>282</v>
       </c>
-      <c r="I2" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H2" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I2" s="6"/>
       <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-    </row>
-    <row r="3" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -9290,13 +9290,13 @@
       <c r="G3" t="s">
         <v>286</v>
       </c>
-      <c r="I3" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H3" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I3" s="6"/>
       <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-    </row>
-    <row r="4" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -9318,13 +9318,13 @@
       <c r="G4" t="s">
         <v>290</v>
       </c>
-      <c r="I4" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H4" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-    </row>
-    <row r="5" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -9346,13 +9346,13 @@
       <c r="G5" t="s">
         <v>294</v>
       </c>
-      <c r="I5" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H5" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I5" s="6"/>
       <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-    </row>
-    <row r="6" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -9374,13 +9374,13 @@
       <c r="G6" t="s">
         <v>298</v>
       </c>
-      <c r="I6" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H6" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I6" s="6"/>
       <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-    </row>
-    <row r="7" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -9402,13 +9402,13 @@
       <c r="G7" t="s">
         <v>302</v>
       </c>
-      <c r="I7" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H7" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I7" s="6"/>
       <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -9430,13 +9430,13 @@
       <c r="G8" t="s">
         <v>306</v>
       </c>
-      <c r="I8" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H8" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I8" s="6"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-    </row>
-    <row r="9" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -9458,13 +9458,13 @@
       <c r="G9" t="s">
         <v>310</v>
       </c>
-      <c r="I9" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H9" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I9" s="6"/>
       <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -9486,13 +9486,13 @@
       <c r="G10" t="s">
         <v>314</v>
       </c>
-      <c r="I10" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H10" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I10" s="6"/>
       <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -9514,13 +9514,13 @@
       <c r="G11" t="s">
         <v>318</v>
       </c>
-      <c r="I11" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H11" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I11" s="6"/>
       <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -9542,13 +9542,13 @@
       <c r="G12" t="s">
         <v>321</v>
       </c>
-      <c r="I12" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H12" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I12" s="6"/>
       <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -9570,13 +9570,13 @@
       <c r="G13" t="s">
         <v>325</v>
       </c>
-      <c r="I13" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H13" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I13" s="6"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -9598,13 +9598,13 @@
       <c r="G14" t="s">
         <v>329</v>
       </c>
-      <c r="I14" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H14" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I14" s="6"/>
       <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-    </row>
-    <row r="15" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -9626,13 +9626,13 @@
       <c r="G15" t="s">
         <v>333</v>
       </c>
-      <c r="I15" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H15" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I15" s="6"/>
       <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -9654,13 +9654,13 @@
       <c r="G16" t="s">
         <v>336</v>
       </c>
-      <c r="I16" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H16" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I16" s="6"/>
       <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-    </row>
-    <row r="17" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -9682,13 +9682,13 @@
       <c r="G17" t="s">
         <v>339</v>
       </c>
-      <c r="I17" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H17" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I17" s="6"/>
       <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-    </row>
-    <row r="18" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -9710,13 +9710,13 @@
       <c r="G18" t="s">
         <v>343</v>
       </c>
-      <c r="I18" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H18" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I18" s="6"/>
       <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-    </row>
-    <row r="19" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -9738,13 +9738,13 @@
       <c r="G19" t="s">
         <v>346</v>
       </c>
-      <c r="I19" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H19" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I19" s="6"/>
       <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-    </row>
-    <row r="20" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -9766,13 +9766,13 @@
       <c r="G20" t="s">
         <v>349</v>
       </c>
-      <c r="I20" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H20" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I20" s="6"/>
       <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-    </row>
-    <row r="21" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -9794,13 +9794,13 @@
       <c r="G21" t="s">
         <v>352</v>
       </c>
-      <c r="I21" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H21" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I21" s="6"/>
       <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-    </row>
-    <row r="22" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -9822,13 +9822,13 @@
       <c r="G22" t="s">
         <v>306</v>
       </c>
-      <c r="I22" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H22" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I22" s="6"/>
       <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-    </row>
-    <row r="23" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -9850,13 +9850,13 @@
       <c r="G23" t="s">
         <v>358</v>
       </c>
-      <c r="I23" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H23" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I23" s="6"/>
       <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-    </row>
-    <row r="24" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -9878,13 +9878,13 @@
       <c r="G24" t="s">
         <v>318</v>
       </c>
-      <c r="I24" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H24" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I24" s="6"/>
       <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-    </row>
-    <row r="25" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -9906,13 +9906,13 @@
       <c r="G25" t="s">
         <v>364</v>
       </c>
-      <c r="I25" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H25" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I25" s="6"/>
       <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-    </row>
-    <row r="26" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -9934,13 +9934,13 @@
       <c r="G26" t="s">
         <v>367</v>
       </c>
-      <c r="I26" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H26" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I26" s="6"/>
       <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-    </row>
-    <row r="27" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -9962,13 +9962,13 @@
       <c r="G27" t="s">
         <v>321</v>
       </c>
-      <c r="I27" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H27" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I27" s="6"/>
       <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-    </row>
-    <row r="28" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -9990,13 +9990,13 @@
       <c r="G28" t="s">
         <v>318</v>
       </c>
-      <c r="I28" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H28" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I28" s="6"/>
       <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-    </row>
-    <row r="29" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -10018,13 +10018,13 @@
       <c r="G29" t="s">
         <v>346</v>
       </c>
-      <c r="I29" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H29" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I29" s="6"/>
       <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-    </row>
-    <row r="30" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -10046,13 +10046,13 @@
       <c r="G30" t="s">
         <v>339</v>
       </c>
-      <c r="I30" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H30" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I30" s="6"/>
       <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-    </row>
-    <row r="31" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -10074,13 +10074,13 @@
       <c r="G31" t="s">
         <v>294</v>
       </c>
-      <c r="I31" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H31" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I31" s="6"/>
       <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-    </row>
-    <row r="32" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
@@ -10102,13 +10102,13 @@
       <c r="G32" t="s">
         <v>380</v>
       </c>
-      <c r="I32" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H32" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I32" s="6"/>
       <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-    </row>
-    <row r="33" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
@@ -10130,13 +10130,13 @@
       <c r="G33" t="s">
         <v>302</v>
       </c>
-      <c r="I33" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H33" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I33" s="6"/>
       <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-    </row>
-    <row r="34" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
@@ -10158,13 +10158,13 @@
       <c r="G34" t="s">
         <v>386</v>
       </c>
-      <c r="I34" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H34" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I34" s="6"/>
       <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-    </row>
-    <row r="35" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
@@ -10186,13 +10186,13 @@
       <c r="G35" t="s">
         <v>389</v>
       </c>
-      <c r="I35" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H35" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I35" s="6"/>
       <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-    </row>
-    <row r="36" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
@@ -10214,13 +10214,13 @@
       <c r="G36" t="s">
         <v>302</v>
       </c>
-      <c r="I36" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H36" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I36" s="6"/>
       <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-    </row>
-    <row r="37" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
@@ -10242,13 +10242,13 @@
       <c r="G37" t="s">
         <v>314</v>
       </c>
-      <c r="I37" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H37" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I37" s="6"/>
       <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-    </row>
-    <row r="38" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
@@ -10270,13 +10270,13 @@
       <c r="G38" t="s">
         <v>282</v>
       </c>
-      <c r="I38" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H38" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I38" s="6"/>
       <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-    </row>
-    <row r="39" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
@@ -10298,13 +10298,13 @@
       <c r="G39" t="s">
         <v>346</v>
       </c>
-      <c r="I39" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H39" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I39" s="6"/>
       <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
-    </row>
-    <row r="40" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
@@ -10326,13 +10326,13 @@
       <c r="G40" t="s">
         <v>325</v>
       </c>
-      <c r="I40" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H40" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I40" s="6"/>
       <c r="J40" s="6"/>
-      <c r="K40" s="6"/>
-    </row>
-    <row r="41" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
@@ -10354,13 +10354,13 @@
       <c r="G41" t="s">
         <v>380</v>
       </c>
-      <c r="I41" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H41" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I41" s="6"/>
       <c r="J41" s="6"/>
-      <c r="K41" s="6"/>
-    </row>
-    <row r="42" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
@@ -10382,13 +10382,13 @@
       <c r="G42" t="s">
         <v>298</v>
       </c>
-      <c r="I42" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H42" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I42" s="6"/>
       <c r="J42" s="6"/>
-      <c r="K42" s="6"/>
-    </row>
-    <row r="43" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>41</v>
       </c>
@@ -10410,13 +10410,13 @@
       <c r="G43" t="s">
         <v>294</v>
       </c>
-      <c r="I43" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H43" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I43" s="6"/>
       <c r="J43" s="6"/>
-      <c r="K43" s="6"/>
-    </row>
-    <row r="44" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>42</v>
       </c>
@@ -10438,13 +10438,13 @@
       <c r="G44" t="s">
         <v>298</v>
       </c>
-      <c r="I44" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H44" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I44" s="6"/>
       <c r="J44" s="6"/>
-      <c r="K44" s="6"/>
-    </row>
-    <row r="45" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>43</v>
       </c>
@@ -10466,13 +10466,13 @@
       <c r="G45" t="s">
         <v>329</v>
       </c>
-      <c r="I45" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H45" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I45" s="6"/>
       <c r="J45" s="6"/>
-      <c r="K45" s="6"/>
-    </row>
-    <row r="46" spans="1:11" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>44</v>
       </c>
@@ -10494,13 +10494,13 @@
       <c r="G46" t="s">
         <v>329</v>
       </c>
-      <c r="I46" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H46" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I46" s="6"/>
       <c r="J46" s="6"/>
-      <c r="K46" s="6"/>
-    </row>
-    <row r="47" spans="1:11" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>45</v>
       </c>
@@ -10522,13 +10522,13 @@
       <c r="G47" t="s">
         <v>329</v>
       </c>
-      <c r="I47" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H47" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I47" s="6"/>
       <c r="J47" s="6"/>
-      <c r="K47" s="6"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>46</v>
       </c>
@@ -10550,13 +10550,13 @@
       <c r="G48" t="s">
         <v>329</v>
       </c>
-      <c r="I48" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H48" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I48" s="6"/>
       <c r="J48" s="6"/>
-      <c r="K48" s="6"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>47</v>
       </c>
@@ -10578,13 +10578,13 @@
       <c r="G49" t="s">
         <v>329</v>
       </c>
-      <c r="I49" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H49" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I49" s="6"/>
       <c r="J49" s="6"/>
-      <c r="K49" s="6"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>48</v>
       </c>
@@ -10606,13 +10606,13 @@
       <c r="G50" t="s">
         <v>329</v>
       </c>
-      <c r="I50" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H50" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I50" s="6"/>
       <c r="J50" s="6"/>
-      <c r="K50" s="6"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>49</v>
       </c>
@@ -10634,13 +10634,13 @@
       <c r="G51" t="s">
         <v>329</v>
       </c>
-      <c r="I51" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H51" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I51" s="6"/>
       <c r="J51" s="6"/>
-      <c r="K51" s="6"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>50</v>
       </c>
@@ -10662,13 +10662,13 @@
       <c r="G52" t="s">
         <v>329</v>
       </c>
-      <c r="I52" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H52" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I52" s="6"/>
       <c r="J52" s="6"/>
-      <c r="K52" s="6"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>51</v>
       </c>
@@ -10690,13 +10690,13 @@
       <c r="G53" t="s">
         <v>329</v>
       </c>
-      <c r="I53" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H53" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I53" s="6"/>
       <c r="J53" s="6"/>
-      <c r="K53" s="6"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>52</v>
       </c>
@@ -10718,13 +10718,13 @@
       <c r="G54" t="s">
         <v>329</v>
       </c>
-      <c r="I54" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H54" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I54" s="6"/>
       <c r="J54" s="6"/>
-      <c r="K54" s="6"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>53</v>
       </c>
@@ -10746,13 +10746,13 @@
       <c r="G55" t="s">
         <v>329</v>
       </c>
-      <c r="I55" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H55" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I55" s="6"/>
       <c r="J55" s="6"/>
-      <c r="K55" s="6"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>54</v>
       </c>
@@ -10774,13 +10774,13 @@
       <c r="G56" t="s">
         <v>329</v>
       </c>
-      <c r="I56" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H56" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I56" s="6"/>
       <c r="J56" s="6"/>
-      <c r="K56" s="6"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>55</v>
       </c>
@@ -10802,13 +10802,13 @@
       <c r="G57" t="s">
         <v>329</v>
       </c>
-      <c r="I57" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H57" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I57" s="6"/>
       <c r="J57" s="6"/>
-      <c r="K57" s="6"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>56</v>
       </c>
@@ -10830,13 +10830,13 @@
       <c r="G58" t="s">
         <v>329</v>
       </c>
-      <c r="I58" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H58" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I58" s="6"/>
       <c r="J58" s="6"/>
-      <c r="K58" s="6"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>57</v>
       </c>
@@ -10858,13 +10858,13 @@
       <c r="G59" t="s">
         <v>329</v>
       </c>
-      <c r="I59" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H59" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I59" s="6"/>
       <c r="J59" s="6"/>
-      <c r="K59" s="6"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>58</v>
       </c>
@@ -10886,13 +10886,13 @@
       <c r="G60" t="s">
         <v>329</v>
       </c>
-      <c r="I60" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H60" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I60" s="6"/>
       <c r="J60" s="6"/>
-      <c r="K60" s="6"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>59</v>
       </c>
@@ -10914,13 +10914,13 @@
       <c r="G61" t="s">
         <v>329</v>
       </c>
-      <c r="I61" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H61" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I61" s="6"/>
       <c r="J61" s="6"/>
-      <c r="K61" s="6"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>60</v>
       </c>
@@ -10942,13 +10942,13 @@
       <c r="G62" t="s">
         <v>329</v>
       </c>
-      <c r="I62" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H62" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I62" s="6"/>
       <c r="J62" s="6"/>
-      <c r="K62" s="6"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>61</v>
       </c>
@@ -10970,16 +10970,16 @@
       <c r="G63" t="s">
         <v>329</v>
       </c>
-      <c r="I63" s="6">
-        <v>42425.375</v>
-      </c>
+      <c r="H63" s="6">
+        <v>42425.375</v>
+      </c>
+      <c r="I63" s="6"/>
       <c r="J63" s="6"/>
-      <c r="K63" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G2556" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -21850,8 +21850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="L114" sqref="L114"/>
+    <sheetView topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="I137" sqref="I137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fix handling of retracted propositions.
</commit_message>
<xml_diff>
--- a/protempa-test-suite/src/test/resources/dsb/sample-data.xlsx
+++ b/protempa-test-suite/src/test/resources/dsb/sample-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arpost/NetBeansProjects/protempa/protempa-test-suite/src/test/resources/dsb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{377A76D0-6E21-434F-A152-25CD8BEA80FB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F59EB8-408D-8645-9746-6E59069D3818}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="537" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="537" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="patient" sheetId="1" r:id="rId1"/>
@@ -9197,8 +9197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10987,7 +10987,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G107"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A92" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -13044,7 +13044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G117"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A91" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -15291,7 +15291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K231"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A211" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -21850,8 +21850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K137"/>
   <sheetViews>
-    <sheetView topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="I137" sqref="I137"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="K115" sqref="K115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>